<commit_message>
working on habitats for CP and HAB
</commit_message>
<xml_diff>
--- a/prep/HAB/hab_wetlands.xlsx
+++ b/prep/HAB/hab_wetlands.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="2160" yWindow="2130" windowWidth="22275" windowHeight="8040"/>
+    <workbookView xWindow="255" yWindow="-270" windowWidth="22275" windowHeight="8040"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="32">
   <si>
     <t>rgn_id</t>
   </si>
@@ -64,13 +64,61 @@
   </si>
   <si>
     <t>Molokai</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>Palustrine_forested_wetland</t>
+  </si>
+  <si>
+    <t>Palustrine_scrub_shrub_wetland</t>
+  </si>
+  <si>
+    <t>Palustrine_emergent_wetland</t>
+  </si>
+  <si>
+    <t>estuarine_forested_wetland</t>
+  </si>
+  <si>
+    <t>esturarine_scrub_shrub_wetland</t>
+  </si>
+  <si>
+    <t>esturarine_emergent_wetland</t>
+  </si>
+  <si>
+    <t>Palustrine Forested Wetland</t>
+  </si>
+  <si>
+    <t>Palustrine Scrub_Shrub Wetland</t>
+  </si>
+  <si>
+    <t>Palustrine Emergent Wetland</t>
+  </si>
+  <si>
+    <t>Estuarine Forest Wetland</t>
+  </si>
+  <si>
+    <t>Estuarine Emergent Wetland</t>
+  </si>
+  <si>
+    <t>Estuarine Scrub_Shrub Wetland</t>
+  </si>
+  <si>
+    <t>Estuarine_Emergent_Wetlands</t>
+  </si>
+  <si>
+    <t>Estuarine_forested_wetland</t>
+  </si>
+  <si>
+    <t>Estuarine_scrub_shrub_wetland</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -80,13 +128,6 @@
     </font>
     <font>
       <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
@@ -117,7 +158,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -420,19 +461,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:F50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" customWidth="1"/>
+    <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -440,16 +482,19 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>4</v>
       </c>
@@ -457,17 +502,20 @@
         <v>6</v>
       </c>
       <c r="C2">
+        <v>2010</v>
+      </c>
+      <c r="D2">
         <v>293852.2</v>
       </c>
-      <c r="D2">
-        <f>C2/(1000000)</f>
+      <c r="E2">
+        <f>D2/(1000000)</f>
         <v>0.29385220000000001</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>4</v>
       </c>
@@ -475,17 +523,20 @@
         <v>6</v>
       </c>
       <c r="C3">
+        <v>2010</v>
+      </c>
+      <c r="D3">
         <v>16289.3</v>
       </c>
-      <c r="D3">
-        <f t="shared" ref="D3:D26" si="0">C3/(1000000)</f>
+      <c r="E3">
+        <f t="shared" ref="E3:E26" si="0">D3/(1000000)</f>
         <v>1.62893E-2</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>4</v>
       </c>
@@ -493,17 +544,20 @@
         <v>6</v>
       </c>
       <c r="C4">
+        <v>2010</v>
+      </c>
+      <c r="D4">
         <v>140855</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <f t="shared" si="0"/>
         <v>0.14085500000000001</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -511,17 +565,20 @@
         <v>7</v>
       </c>
       <c r="C5">
+        <v>2010</v>
+      </c>
+      <c r="D5">
         <v>1846880.6</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <f t="shared" si="0"/>
         <v>1.8468806</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
@@ -529,17 +586,20 @@
         <v>7</v>
       </c>
       <c r="C6">
+        <v>2010</v>
+      </c>
+      <c r="D6">
         <v>707305</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <f t="shared" si="0"/>
         <v>0.70730499999999996</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
@@ -547,17 +607,20 @@
         <v>7</v>
       </c>
       <c r="C7">
+        <v>2010</v>
+      </c>
+      <c r="D7">
         <v>669991.69999999995</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <f t="shared" si="0"/>
         <v>0.66999169999999997</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2</v>
       </c>
@@ -565,17 +628,20 @@
         <v>8</v>
       </c>
       <c r="C8">
+        <v>2010</v>
+      </c>
+      <c r="D8">
         <v>1930389.1</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <f t="shared" si="0"/>
         <v>1.9303891000000002</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2</v>
       </c>
@@ -583,17 +649,20 @@
         <v>8</v>
       </c>
       <c r="C9">
+        <v>2010</v>
+      </c>
+      <c r="D9">
         <v>2060190.7</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <f t="shared" si="0"/>
         <v>2.0601907000000002</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2</v>
       </c>
@@ -601,17 +670,20 @@
         <v>8</v>
       </c>
       <c r="C10">
+        <v>2010</v>
+      </c>
+      <c r="D10">
         <v>2334948.5</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <f t="shared" si="0"/>
         <v>2.3349484999999999</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1</v>
       </c>
@@ -619,17 +691,20 @@
         <v>9</v>
       </c>
       <c r="C11">
+        <v>2010</v>
+      </c>
+      <c r="D11">
         <v>48297.599999999999</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <f t="shared" si="0"/>
         <v>4.8297599999999996E-2</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1</v>
       </c>
@@ -637,17 +712,20 @@
         <v>9</v>
       </c>
       <c r="C12">
+        <v>2010</v>
+      </c>
+      <c r="D12">
         <v>973.4</v>
       </c>
-      <c r="D12">
+      <c r="E12">
         <f t="shared" si="0"/>
         <v>9.7340000000000002E-4</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1</v>
       </c>
@@ -655,17 +733,20 @@
         <v>9</v>
       </c>
       <c r="C13">
+        <v>2010</v>
+      </c>
+      <c r="D13">
         <v>115585.9</v>
       </c>
-      <c r="D13">
+      <c r="E13">
         <f t="shared" si="0"/>
         <v>0.11558589999999999</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2</v>
       </c>
@@ -673,17 +754,20 @@
         <v>8</v>
       </c>
       <c r="C14">
+        <v>2010</v>
+      </c>
+      <c r="D14">
         <v>972587.52000000002</v>
       </c>
-      <c r="D14">
+      <c r="E14">
         <f t="shared" si="0"/>
         <v>0.97258752000000004</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2</v>
       </c>
@@ -691,17 +775,20 @@
         <v>8</v>
       </c>
       <c r="C15">
+        <v>2010</v>
+      </c>
+      <c r="D15">
         <v>956096.6</v>
       </c>
-      <c r="D15">
+      <c r="E15">
         <f t="shared" si="0"/>
         <v>0.95609659999999996</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2</v>
       </c>
@@ -709,17 +796,20 @@
         <v>8</v>
       </c>
       <c r="C16">
+        <v>2010</v>
+      </c>
+      <c r="D16">
         <v>1517938.6</v>
       </c>
-      <c r="D16">
+      <c r="E16">
         <f t="shared" si="0"/>
         <v>1.5179386000000001</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>4</v>
       </c>
@@ -727,17 +817,20 @@
         <v>6</v>
       </c>
       <c r="C17">
+        <v>2010</v>
+      </c>
+      <c r="D17">
         <v>1448956.8</v>
       </c>
-      <c r="D17">
+      <c r="E17">
         <f t="shared" si="0"/>
         <v>1.4489568000000002</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>4</v>
       </c>
@@ -745,17 +838,20 @@
         <v>6</v>
       </c>
       <c r="C18">
+        <v>2010</v>
+      </c>
+      <c r="D18">
         <v>390873.59999999998</v>
       </c>
-      <c r="D18">
+      <c r="E18">
         <f t="shared" si="0"/>
         <v>0.39087359999999999</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>4</v>
       </c>
@@ -763,17 +859,20 @@
         <v>6</v>
       </c>
       <c r="C19">
+        <v>2010</v>
+      </c>
+      <c r="D19">
         <v>1515386.9</v>
       </c>
-      <c r="D19">
+      <c r="E19">
         <f t="shared" si="0"/>
         <v>1.5153869</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>3</v>
       </c>
@@ -781,17 +880,20 @@
         <v>7</v>
       </c>
       <c r="C20">
+        <v>2010</v>
+      </c>
+      <c r="D20">
         <v>700243.2</v>
       </c>
-      <c r="D20">
+      <c r="E20">
         <f t="shared" si="0"/>
         <v>0.70024319999999995</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>3</v>
       </c>
@@ -799,17 +901,20 @@
         <v>7</v>
       </c>
       <c r="C21">
+        <v>2010</v>
+      </c>
+      <c r="D21">
         <v>678257.3</v>
       </c>
-      <c r="D21">
+      <c r="E21">
         <f t="shared" si="0"/>
         <v>0.67825730000000006</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>3</v>
       </c>
@@ -817,17 +922,20 @@
         <v>7</v>
       </c>
       <c r="C22">
+        <v>2010</v>
+      </c>
+      <c r="D22">
         <v>2142063.6</v>
       </c>
-      <c r="D22">
+      <c r="E22">
         <f t="shared" si="0"/>
         <v>2.1420636000000002</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2</v>
       </c>
@@ -835,17 +943,20 @@
         <v>6</v>
       </c>
       <c r="C23">
+        <v>2010</v>
+      </c>
+      <c r="D23">
         <v>5316.48</v>
       </c>
-      <c r="D23">
+      <c r="E23">
         <f t="shared" si="0"/>
         <v>5.3164799999999993E-3</v>
       </c>
-      <c r="E23" t="s">
+      <c r="F23" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>2</v>
       </c>
@@ -853,17 +964,20 @@
         <v>15</v>
       </c>
       <c r="C24">
+        <v>2010</v>
+      </c>
+      <c r="D24">
         <v>1246475.5</v>
       </c>
-      <c r="D24">
+      <c r="E24">
         <f t="shared" si="0"/>
         <v>1.2464755000000001</v>
       </c>
-      <c r="E24" t="s">
+      <c r="F24" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2</v>
       </c>
@@ -871,17 +985,20 @@
         <v>15</v>
       </c>
       <c r="C25">
+        <v>2010</v>
+      </c>
+      <c r="D25">
         <v>576616.30000000005</v>
       </c>
-      <c r="D25">
+      <c r="E25">
         <f t="shared" si="0"/>
         <v>0.57661630000000008</v>
       </c>
-      <c r="E25" t="s">
+      <c r="F25" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2</v>
       </c>
@@ -889,14 +1006,521 @@
         <v>15</v>
       </c>
       <c r="C26">
+        <v>2010</v>
+      </c>
+      <c r="D26">
         <v>272062.09999999998</v>
       </c>
-      <c r="D26">
+      <c r="E26">
         <f t="shared" si="0"/>
         <v>0.27206209999999997</v>
       </c>
-      <c r="E26" t="s">
+      <c r="F26" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>1</v>
+      </c>
+      <c r="B27" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27">
+        <v>2005</v>
+      </c>
+      <c r="D27">
+        <v>681286.5</v>
+      </c>
+      <c r="E27">
+        <f>D27/1000000</f>
+        <v>0.68128650000000002</v>
+      </c>
+      <c r="F27" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>1</v>
+      </c>
+      <c r="B28" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28">
+        <v>2005</v>
+      </c>
+      <c r="D28">
+        <v>451791.02</v>
+      </c>
+      <c r="E28">
+        <f t="shared" ref="E28:E50" si="1">D28/1000000</f>
+        <v>0.45179102000000004</v>
+      </c>
+      <c r="F28" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>1</v>
+      </c>
+      <c r="B29" t="s">
+        <v>9</v>
+      </c>
+      <c r="C29">
+        <v>2005</v>
+      </c>
+      <c r="D29">
+        <v>967480.8</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="1"/>
+        <v>0.96748080000000003</v>
+      </c>
+      <c r="F29" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>1</v>
+      </c>
+      <c r="B30" t="s">
+        <v>9</v>
+      </c>
+      <c r="C30">
+        <v>2005</v>
+      </c>
+      <c r="D30">
+        <v>50399</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="1"/>
+        <v>5.0398999999999999E-2</v>
+      </c>
+      <c r="F30" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>1</v>
+      </c>
+      <c r="B31" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31">
+        <v>2005</v>
+      </c>
+      <c r="D31">
+        <v>900</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="1"/>
+        <v>8.9999999999999998E-4</v>
+      </c>
+      <c r="F31" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>1</v>
+      </c>
+      <c r="B32" t="s">
+        <v>9</v>
+      </c>
+      <c r="C32">
+        <v>2005</v>
+      </c>
+      <c r="D32">
+        <v>120598</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="1"/>
+        <v>0.120598</v>
+      </c>
+      <c r="F32" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>4</v>
+      </c>
+      <c r="B33" t="s">
+        <v>6</v>
+      </c>
+      <c r="C33">
+        <v>2005</v>
+      </c>
+      <c r="D33">
+        <v>1248275.2</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="1"/>
+        <v>1.2482751999999999</v>
+      </c>
+      <c r="F33" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>4</v>
+      </c>
+      <c r="B34" t="s">
+        <v>6</v>
+      </c>
+      <c r="C34">
+        <v>2005</v>
+      </c>
+      <c r="D34">
+        <v>304194</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="1"/>
+        <v>0.30419400000000002</v>
+      </c>
+      <c r="F34" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>4</v>
+      </c>
+      <c r="B35" t="s">
+        <v>6</v>
+      </c>
+      <c r="C35">
+        <v>2005</v>
+      </c>
+      <c r="D35">
+        <v>1495770.3</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="1"/>
+        <v>1.4957703</v>
+      </c>
+      <c r="F35" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>4</v>
+      </c>
+      <c r="B36" t="s">
+        <v>6</v>
+      </c>
+      <c r="C36">
+        <v>2005</v>
+      </c>
+      <c r="D36">
+        <v>230395.4</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="1"/>
+        <v>0.2303954</v>
+      </c>
+      <c r="F36" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>4</v>
+      </c>
+      <c r="B37" t="s">
+        <v>6</v>
+      </c>
+      <c r="C37">
+        <v>2005</v>
+      </c>
+      <c r="D37">
+        <v>25199.5</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="1"/>
+        <v>2.51995E-2</v>
+      </c>
+      <c r="F37" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>4</v>
+      </c>
+      <c r="B38" t="s">
+        <v>6</v>
+      </c>
+      <c r="C38">
+        <v>2005</v>
+      </c>
+      <c r="D38">
+        <v>98098.1</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="1"/>
+        <v>9.8098100000000008E-2</v>
+      </c>
+      <c r="F38" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>2</v>
+      </c>
+      <c r="B39" t="s">
+        <v>8</v>
+      </c>
+      <c r="C39">
+        <v>2005</v>
+      </c>
+      <c r="D39">
+        <v>3568500</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="1"/>
+        <v>3.5684999999999998</v>
+      </c>
+      <c r="F39" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>2</v>
+      </c>
+      <c r="B40" t="s">
+        <v>8</v>
+      </c>
+      <c r="C40">
+        <v>2005</v>
+      </c>
+      <c r="D40">
+        <v>1709100</v>
+      </c>
+      <c r="E40">
+        <f t="shared" si="1"/>
+        <v>1.7091000000000001</v>
+      </c>
+      <c r="F40" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>2</v>
+      </c>
+      <c r="B41" t="s">
+        <v>8</v>
+      </c>
+      <c r="C41">
+        <v>2005</v>
+      </c>
+      <c r="D41">
+        <v>1440000</v>
+      </c>
+      <c r="E41">
+        <f t="shared" si="1"/>
+        <v>1.44</v>
+      </c>
+      <c r="F41" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>2</v>
+      </c>
+      <c r="B42" t="s">
+        <v>8</v>
+      </c>
+      <c r="C42">
+        <v>2005</v>
+      </c>
+      <c r="D42">
+        <v>369000</v>
+      </c>
+      <c r="E42">
+        <f t="shared" si="1"/>
+        <v>0.36899999999999999</v>
+      </c>
+      <c r="F42" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>2</v>
+      </c>
+      <c r="B43" t="s">
+        <v>8</v>
+      </c>
+      <c r="C43">
+        <v>2005</v>
+      </c>
+      <c r="D43">
+        <v>16200</v>
+      </c>
+      <c r="E43">
+        <f t="shared" si="1"/>
+        <v>1.6199999999999999E-2</v>
+      </c>
+      <c r="F43" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>2</v>
+      </c>
+      <c r="B44" t="s">
+        <v>8</v>
+      </c>
+      <c r="C44">
+        <v>2005</v>
+      </c>
+      <c r="D44">
+        <v>38505940.5</v>
+      </c>
+      <c r="E44">
+        <f t="shared" si="1"/>
+        <v>38.505940500000001</v>
+      </c>
+      <c r="F44" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>3</v>
+      </c>
+      <c r="B45" t="s">
+        <v>7</v>
+      </c>
+      <c r="C45">
+        <v>2005</v>
+      </c>
+      <c r="D45">
+        <v>2314753.98</v>
+      </c>
+      <c r="E45">
+        <f t="shared" si="1"/>
+        <v>2.3147539799999999</v>
+      </c>
+      <c r="F45" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>3</v>
+      </c>
+      <c r="B46" t="s">
+        <v>7</v>
+      </c>
+      <c r="C46">
+        <v>2005</v>
+      </c>
+      <c r="D46">
+        <v>1191576.3</v>
+      </c>
+      <c r="E46">
+        <f t="shared" si="1"/>
+        <v>1.1915763000000001</v>
+      </c>
+      <c r="F46" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>3</v>
+      </c>
+      <c r="B47" t="s">
+        <v>7</v>
+      </c>
+      <c r="C47">
+        <v>2005</v>
+      </c>
+      <c r="D47">
+        <v>395992.12</v>
+      </c>
+      <c r="E47">
+        <f t="shared" si="1"/>
+        <v>0.39599212</v>
+      </c>
+      <c r="F47" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>3</v>
+      </c>
+      <c r="B48" t="s">
+        <v>7</v>
+      </c>
+      <c r="C48">
+        <v>2005</v>
+      </c>
+      <c r="D48">
+        <v>467990.7</v>
+      </c>
+      <c r="E48">
+        <f t="shared" si="1"/>
+        <v>0.46799070000000004</v>
+      </c>
+      <c r="F48" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>3</v>
+      </c>
+      <c r="B49" t="s">
+        <v>7</v>
+      </c>
+      <c r="C49">
+        <v>2005</v>
+      </c>
+      <c r="D49">
+        <v>779384.5</v>
+      </c>
+      <c r="E49">
+        <f t="shared" si="1"/>
+        <v>0.77938450000000004</v>
+      </c>
+      <c r="F49" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>3</v>
+      </c>
+      <c r="B50" t="s">
+        <v>7</v>
+      </c>
+      <c r="C50">
+        <v>2005</v>
+      </c>
+      <c r="D50">
+        <v>4441411.7</v>
+      </c>
+      <c r="E50">
+        <f t="shared" si="1"/>
+        <v>4.4414117000000006</v>
+      </c>
+      <c r="F50" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>